<commit_message>
add: add cls model code
</commit_message>
<xml_diff>
--- a/src/Output/ML_All/Tx(K)_ml.xlsx
+++ b/src/Output/ML_All/Tx(K)_ml.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>XGBRegressor</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>edRVFL</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -508,7 +513,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>{'max_depth': None, 'n_estimators': 200}</t>
+          <t>{'max_depth': 20, 'n_estimators': 100}</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -529,6 +534,11 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 500}</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>{'activation': 'relu', 'b_random_vec_range': [0, 10], 'lam': 1, 'n_layer': 16, 'n_nodes': 256, 'random_seed': 358, 'same_feature': True, 'w_random_vec_range': [-10, 10]}</t>
         </is>
       </c>
     </row>
@@ -551,19 +561,22 @@
         <v>0.07614074535858557</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05300022931316997</v>
+        <v>0.05290137422467665</v>
       </c>
       <c r="G3" t="n">
-        <v>0.05016210139375073</v>
+        <v>0.05019867482937072</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1009816767629359</v>
+        <v>0.1015212474423683</v>
       </c>
       <c r="I3" t="n">
         <v>0.04719998031908251</v>
       </c>
       <c r="J3" t="n">
         <v>0.05070881903069058</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.02673389891972606</v>
       </c>
     </row>
     <row r="4">
@@ -585,19 +598,22 @@
         <v>0.8988318188252457</v>
       </c>
       <c r="F4" t="n">
-        <v>0.948271590950859</v>
+        <v>0.9483827196779414</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9537287723833089</v>
+        <v>0.953396796924791</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8241523719504054</v>
+        <v>0.8230625889627975</v>
       </c>
       <c r="I4" t="n">
         <v>0.9595943643042307</v>
       </c>
       <c r="J4" t="n">
         <v>0.9542264983691717</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.986653353629201</v>
       </c>
     </row>
     <row r="5">
@@ -619,19 +635,22 @@
         <v>16.13094892244744</v>
       </c>
       <c r="F5" t="n">
-        <v>6.427079871195701</v>
+        <v>6.427331223082751</v>
       </c>
       <c r="G5" t="n">
-        <v>6.261983639660482</v>
+        <v>6.371517571339483</v>
       </c>
       <c r="H5" t="n">
-        <v>20.09648579063794</v>
+        <v>19.40265142933292</v>
       </c>
       <c r="I5" t="n">
         <v>6.296702272859105</v>
       </c>
       <c r="J5" t="n">
         <v>7.175632936858507</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3.774573562720013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>